<commit_message>
new bgp experiment #6
</commit_message>
<xml_diff>
--- a/binary_growth_phenotypes/metadata/binary_growth_research.xlsx
+++ b/binary_growth_phenotypes/metadata/binary_growth_research.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baeuerle/Organisation/Masterarbeit/C_striatum_wetlab/growth_binary/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baeuerle/Organisation/Masterarbeit/C_striatum_wetlab/binary_growth_phenotypes/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1799C4C3-EF1B-7747-B7C0-ADEA9A561AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9A33FC-46C0-8243-920D-7405266AD43B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="additives" sheetId="1" r:id="rId1"/>
@@ -260,7 +260,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="#,##0.00000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -335,13 +335,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -650,7 +650,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>